<commit_message>
error changes to add reset button
</commit_message>
<xml_diff>
--- a/generated_timesheets/January_2025_Timesheet_Shamik.xlsx
+++ b/generated_timesheets/January_2025_Timesheet_Shamik.xlsx
@@ -709,17 +709,17 @@
           <t>02-January-2025</t>
         </is>
       </c>
-      <c r="C12" s="10" t="inlineStr">
-        <is>
-          <t>1.0</t>
-        </is>
-      </c>
+      <c r="C12" s="10" t="inlineStr"/>
       <c r="D12" s="12" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
-      <c r="E12" s="10" t="inlineStr"/>
+      <c r="E12" s="10" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
       <c r="F12" s="10" t="inlineStr"/>
       <c r="G12" s="10" t="inlineStr"/>
       <c r="H12" s="13" t="inlineStr">
@@ -737,17 +737,17 @@
           <t>03-January-2025</t>
         </is>
       </c>
-      <c r="C13" s="10" t="inlineStr">
-        <is>
-          <t>1.0</t>
-        </is>
-      </c>
+      <c r="C13" s="10" t="inlineStr"/>
       <c r="D13" s="12" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
-      <c r="E13" s="10" t="inlineStr"/>
+      <c r="E13" s="10" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
       <c r="F13" s="10" t="inlineStr"/>
       <c r="G13" s="10" t="inlineStr"/>
       <c r="H13" s="13" t="inlineStr">
@@ -1514,7 +1514,7 @@
       </c>
       <c r="C44" s="16" t="inlineStr">
         <is>
-          <t>20.0</t>
+          <t>18.0</t>
         </is>
       </c>
       <c r="D44" s="16" t="inlineStr">
@@ -1524,7 +1524,7 @@
       </c>
       <c r="E44" s="16" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>2.0</t>
         </is>
       </c>
       <c r="F44" s="16" t="inlineStr">
@@ -1576,7 +1576,7 @@
       </c>
       <c r="B48" s="17" t="inlineStr">
         <is>
-          <t>08 - February - 2025</t>
+          <t>09 - February - 2025</t>
         </is>
       </c>
       <c r="H48" s="14" t="n"/>

</xml_diff>